<commit_message>
Update Admin Task List & Summary (1).xlsx
</commit_message>
<xml_diff>
--- a/docs/Admin Task List & Summary (1).xlsx
+++ b/docs/Admin Task List & Summary (1).xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="174">
   <si>
     <t xml:space="preserve">Sr. NO </t>
   </si>
@@ -3061,7 +3061,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D109" sqref="D109"/>
+      <selection pane="bottomLeft" activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5349,11 +5349,9 @@
       <c r="D102" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>9</v>
+      <c r="E102" s="1"/>
+      <c r="F102" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -5372,8 +5370,8 @@
         <v>17</v>
       </c>
       <c r="E103" s="1"/>
-      <c r="F103" s="1" t="s">
-        <v>9</v>
+      <c r="F103" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>

</xml_diff>